<commit_message>
Corrigido erros de digitação
</commit_message>
<xml_diff>
--- a/17-  Análise de Eventos para cada Cenário.xlsx
+++ b/17-  Análise de Eventos para cada Cenário.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alisson A. Alves\Desktop\Faculdade\2º Semestre\Engenharia de Software\Nossos_artefatos\Engenharia_de_software-TPD_Grafica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77929823-52C1-44FD-B4F9-0898424FA99C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D586B724-2B2E-47D0-ACB1-1693E0EB0D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="31">
   <si>
     <t>Capacidade</t>
   </si>
@@ -81,9 +81,6 @@
     <t xml:space="preserve">Recusar pagamento </t>
   </si>
   <si>
-    <t>Produto pronto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Entregar produto </t>
   </si>
   <si>
@@ -109,6 +106,18 @@
   </si>
   <si>
     <t>x(2)</t>
+  </si>
+  <si>
+    <t>x(4)</t>
+  </si>
+  <si>
+    <t>x(5)</t>
+  </si>
+  <si>
+    <t>Retirar produto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entrega do produto </t>
   </si>
 </sst>
 </file>
@@ -132,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,6 +178,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -326,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,6 +421,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -746,10 +767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B64D5539-9B1C-47CB-A706-259A5CF84E4F}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,12 +822,12 @@
       <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="23" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -819,13 +840,13 @@
       <c r="C3" s="14">
         <v>2</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="9"/>
       <c r="G3" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -839,22 +860,84 @@
       <c r="C4" s="20">
         <v>3</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="23" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="9"/>
       <c r="G4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="13">
+        <v>4</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="14">
+        <v>5</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="20">
+        <v>6</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -865,7 +948,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,7 +1088,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+      <selection activeCell="A2" sqref="A2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1198,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1242,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>10</v>
@@ -1168,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="15"/>
       <c r="F2" s="5"/>
@@ -1186,7 +1269,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1252,7 +1335,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>10</v>
@@ -1261,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -1277,7 +1360,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1295,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1318,7 +1401,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,7 +1445,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>10</v>

</xml_diff>